<commit_message>
started making the game, also fixed some bugs in the framework and added some methods to Entity class
</commit_message>
<xml_diff>
--- a/packs_file.xlsx
+++ b/packs_file.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="trunk" sheetId="1" r:id="rId1"/>
     <sheet name="frog" sheetId="4" r:id="rId2"/>
+    <sheet name="Start menu button" sheetId="6" r:id="rId3"/>
+    <sheet name="Dot" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -58,6 +60,18 @@
   </si>
   <si>
     <t>time</t>
+  </si>
+  <si>
+    <t>illustrations/start menu button.png</t>
+  </si>
+  <si>
+    <t>Start menu button</t>
+  </si>
+  <si>
+    <t>Dot</t>
+  </si>
+  <si>
+    <t>illustrations/dot.png</t>
   </si>
 </sst>
 </file>
@@ -455,7 +469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -516,4 +530,138 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>400</v>
+      </c>
+      <c r="E2">
+        <v>80</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
almost fineshed the local multiplayer game added some functions and fixed some bug in the framework while making the game
</commit_message>
<xml_diff>
--- a/packs_file.xlsx
+++ b/packs_file.xlsx
@@ -9,13 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="trunk" sheetId="1" r:id="rId1"/>
-    <sheet name="frog" sheetId="4" r:id="rId2"/>
-    <sheet name="Start menu button" sheetId="6" r:id="rId3"/>
-    <sheet name="Dot" sheetId="7" r:id="rId4"/>
+    <sheet name="Start menu button" sheetId="6" r:id="rId1"/>
+    <sheet name="Dot" sheetId="7" r:id="rId2"/>
+    <sheet name="Line" sheetId="9" r:id="rId3"/>
+    <sheet name="Square" sheetId="10" r:id="rId4"/>
+    <sheet name="Layout" sheetId="11" r:id="rId5"/>
+    <sheet name="Card" sheetId="13" r:id="rId6"/>
+    <sheet name="Frog" sheetId="4" r:id="rId7"/>
+    <sheet name="Snowy" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -47,18 +51,9 @@
     <t>loop</t>
   </si>
   <si>
-    <t>speed</t>
-  </si>
-  <si>
     <t>happy</t>
   </si>
   <si>
-    <t>animations/human idle.png</t>
-  </si>
-  <si>
-    <t>animations/happy trunk.png</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
@@ -72,6 +67,105 @@
   </si>
   <si>
     <t>illustrations/dot.png</t>
+  </si>
+  <si>
+    <t>illustrations/black horizontal line.png</t>
+  </si>
+  <si>
+    <t>black hl</t>
+  </si>
+  <si>
+    <t>gray hl</t>
+  </si>
+  <si>
+    <t>illustrations/gray horizontal line.png</t>
+  </si>
+  <si>
+    <t>black vl</t>
+  </si>
+  <si>
+    <t>gray vl</t>
+  </si>
+  <si>
+    <t>illustrations/black vertical line.png</t>
+  </si>
+  <si>
+    <t>illustrations/gray vertical line.png</t>
+  </si>
+  <si>
+    <t>color 1</t>
+  </si>
+  <si>
+    <t>color 2</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>illustrations/empty square.png</t>
+  </si>
+  <si>
+    <t>illustrations/square color 1.png</t>
+  </si>
+  <si>
+    <t>illustrations/square color 2.png</t>
+  </si>
+  <si>
+    <t>illustrations/empty vertical line.png</t>
+  </si>
+  <si>
+    <t>illustrations/empty horizontal line.png</t>
+  </si>
+  <si>
+    <t>empty hl</t>
+  </si>
+  <si>
+    <t>empty vl</t>
+  </si>
+  <si>
+    <t>regular</t>
+  </si>
+  <si>
+    <t>animations/frog happy.png</t>
+  </si>
+  <si>
+    <t>shadow</t>
+  </si>
+  <si>
+    <t>animations/frog shadow.png</t>
+  </si>
+  <si>
+    <t>animations/frog regular.png</t>
+  </si>
+  <si>
+    <t>layout</t>
+  </si>
+  <si>
+    <t>illustrations/layout.png</t>
+  </si>
+  <si>
+    <t>illustrations/card frog.png</t>
+  </si>
+  <si>
+    <t>frog</t>
+  </si>
+  <si>
+    <t>illustrations/card empty.png</t>
+  </si>
+  <si>
+    <t>animations/snowy regular.png</t>
+  </si>
+  <si>
+    <t>animations/snowy shadow.png</t>
+  </si>
+  <si>
+    <t>animations/snowy happy.png</t>
+  </si>
+  <si>
+    <t>snowy</t>
+  </si>
+  <si>
+    <t>illustrations/card snowy.png</t>
   </si>
 </sst>
 </file>
@@ -403,140 +497,6 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="20.625" customWidth="1"/>
-    <col min="2" max="2" width="60.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>32</v>
-      </c>
-      <c r="E2">
-        <v>32</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>PROPER(TRUE)</f>
-        <v>True</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="20.625" customWidth="1"/>
-    <col min="2" max="2" width="60.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>64</v>
-      </c>
-      <c r="E2">
-        <v>64</v>
-      </c>
-      <c r="F2">
-        <v>0.1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>PROPER(TRUE)</f>
-        <v>True</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
@@ -563,7 +523,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -571,10 +531,10 @@
     </row>
     <row r="2" spans="1:7" ht="16.5">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -599,11 +559,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -630,7 +590,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -638,10 +598,10 @@
     </row>
     <row r="2" spans="1:7" ht="16.5">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -656,6 +616,753 @@
         <v>0.1</v>
       </c>
       <c r="G2" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>66</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G7" si="0">PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>66</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>66</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>66</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16.5">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>66</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.5">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>66</v>
+      </c>
+      <c r="F7">
+        <v>0.1</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>True</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="A2:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>69</v>
+      </c>
+      <c r="E2">
+        <v>69</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>69</v>
+      </c>
+      <c r="E3">
+        <v>69</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>69</v>
+      </c>
+      <c r="E4">
+        <v>69</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.5">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5">
+      <c r="B7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1920</v>
+      </c>
+      <c r="E2">
+        <v>1080</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.5">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5">
+      <c r="B7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>550</v>
+      </c>
+      <c r="E2">
+        <v>851</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>550</v>
+      </c>
+      <c r="E3">
+        <v>851</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>550</v>
+      </c>
+      <c r="E4">
+        <v>851</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.5">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5">
+      <c r="B7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>64</v>
+      </c>
+      <c r="E2">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>64</v>
+      </c>
+      <c r="E4">
+        <v>64</v>
+      </c>
+      <c r="F4">
+        <v>0.08</v>
+      </c>
+      <c r="G4" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>64</v>
+      </c>
+      <c r="E2">
+        <v>64</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>64</v>
+      </c>
+      <c r="E4">
+        <v>64</v>
+      </c>
+      <c r="F4">
+        <v>0.08</v>
+      </c>
+      <c r="G4" t="str">
         <f>PROPER(TRUE)</f>
         <v>True</v>
       </c>

</xml_diff>

<commit_message>
fixed scaling function in the framework and other bugs and added new stuf to the game
</commit_message>
<xml_diff>
--- a/packs_file.xlsx
+++ b/packs_file.xlsx
@@ -20,6 +20,7 @@
     <sheet name="Card" sheetId="13" r:id="rId6"/>
     <sheet name="Frog" sheetId="4" r:id="rId7"/>
     <sheet name="Snowy" sheetId="14" r:id="rId8"/>
+    <sheet name="Chick" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="51">
   <si>
     <t>name</t>
   </si>
@@ -153,9 +154,6 @@
     <t>illustrations/card empty.png</t>
   </si>
   <si>
-    <t>animations/snowy regular.png</t>
-  </si>
-  <si>
     <t>animations/snowy shadow.png</t>
   </si>
   <si>
@@ -166,6 +164,27 @@
   </si>
   <si>
     <t>illustrations/card snowy.png</t>
+  </si>
+  <si>
+    <t>animations/snowy sad.png</t>
+  </si>
+  <si>
+    <t>sad</t>
+  </si>
+  <si>
+    <t>animations/chick shadow.png</t>
+  </si>
+  <si>
+    <t>animations/chick regular.png</t>
+  </si>
+  <si>
+    <t>animations/chick happy.png</t>
+  </si>
+  <si>
+    <t>chick</t>
+  </si>
+  <si>
+    <t>illustrations/card chick.png</t>
   </si>
 </sst>
 </file>
@@ -564,73 +583,6 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="20.625" customWidth="1"/>
-    <col min="2" max="2" width="60.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>0.1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>PROPER(TRUE)</f>
-        <v>True</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -665,6 +617,73 @@
     </row>
     <row r="2" spans="1:7" ht="16.5">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -683,7 +702,7 @@
         <v>0.1</v>
       </c>
       <c r="G2" t="str">
-        <f t="shared" ref="G2:G7" si="0">PROPER(TRUE)</f>
+        <f t="shared" ref="G2:G6" si="0">PROPER(TRUE)</f>
         <v>True</v>
       </c>
     </row>
@@ -719,7 +738,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>66</v>
@@ -728,11 +747,11 @@
         <v>4</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="0"/>
-        <v>True</v>
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16.5">
@@ -791,7 +810,7 @@
         <v>18</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -800,11 +819,11 @@
         <v>66</v>
       </c>
       <c r="F7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="0"/>
-        <v>True</v>
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
       </c>
     </row>
   </sheetData>
@@ -1024,6 +1043,381 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>550</v>
+      </c>
+      <c r="E2">
+        <v>851</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>550</v>
+      </c>
+      <c r="E3">
+        <v>851</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>550</v>
+      </c>
+      <c r="E4">
+        <v>851</v>
+      </c>
+      <c r="F4">
+        <v>0.1</v>
+      </c>
+      <c r="G4" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16.5">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>550</v>
+      </c>
+      <c r="E5">
+        <v>851</v>
+      </c>
+      <c r="F5">
+        <v>0.1</v>
+      </c>
+      <c r="G5" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="16.5">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5">
+      <c r="B7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>128</v>
+      </c>
+      <c r="E2">
+        <v>128</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>128</v>
+      </c>
+      <c r="E3">
+        <v>128</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>128</v>
+      </c>
+      <c r="E4">
+        <v>128</v>
+      </c>
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="60.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>128</v>
+      </c>
+      <c r="E2">
+        <v>128</v>
+      </c>
+      <c r="F2">
+        <v>0.1</v>
+      </c>
+      <c r="G2" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>128</v>
+      </c>
+      <c r="E3">
+        <v>128</v>
+      </c>
+      <c r="F3">
+        <v>0.1</v>
+      </c>
+      <c r="G3" t="str">
+        <f>PROPER(FALSE)</f>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="16.5">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>128</v>
+      </c>
+      <c r="E4">
+        <v>128</v>
+      </c>
+      <c r="F4">
+        <v>0.2</v>
+      </c>
+      <c r="G4" t="str">
+        <f>PROPER(TRUE)</f>
+        <v>True</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1058,19 +1452,19 @@
     </row>
     <row r="2" spans="1:7" ht="16.5">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>550</v>
+        <v>128</v>
       </c>
       <c r="E2">
-        <v>851</v>
+        <v>128</v>
       </c>
       <c r="F2">
         <v>0.1</v>
@@ -1082,19 +1476,19 @@
     </row>
     <row r="3" spans="1:7" ht="16.5">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>550</v>
+        <v>128</v>
       </c>
       <c r="E3">
-        <v>851</v>
+        <v>128</v>
       </c>
       <c r="F3">
         <v>0.1</v>
@@ -1106,261 +1500,22 @@
     </row>
     <row r="4" spans="1:7" ht="16.5">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D4">
-        <v>550</v>
+        <v>128</v>
       </c>
       <c r="E4">
-        <v>851</v>
+        <v>128</v>
       </c>
       <c r="F4">
-        <v>0.1</v>
-      </c>
-      <c r="G4" t="str">
-        <f>PROPER(FALSE)</f>
-        <v>False</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16.5">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="16.5">
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" ht="16.5">
-      <c r="B7" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="20.625" customWidth="1"/>
-    <col min="2" max="2" width="60.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>64</v>
-      </c>
-      <c r="E2">
-        <v>64</v>
-      </c>
-      <c r="F2">
-        <v>0.1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>PROPER(FALSE)</f>
-        <v>False</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>64</v>
-      </c>
-      <c r="E3">
-        <v>64</v>
-      </c>
-      <c r="F3">
-        <v>0.1</v>
-      </c>
-      <c r="G3" t="str">
-        <f>PROPER(FALSE)</f>
-        <v>False</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16.5">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>64</v>
-      </c>
-      <c r="E4">
-        <v>64</v>
-      </c>
-      <c r="F4">
-        <v>0.08</v>
-      </c>
-      <c r="G4" t="str">
-        <f>PROPER(TRUE)</f>
-        <v>True</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="20.625" customWidth="1"/>
-    <col min="2" max="2" width="60.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="16.5">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>64</v>
-      </c>
-      <c r="E2">
-        <v>64</v>
-      </c>
-      <c r="F2">
-        <v>0.1</v>
-      </c>
-      <c r="G2" t="str">
-        <f>PROPER(FALSE)</f>
-        <v>False</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>64</v>
-      </c>
-      <c r="E3">
-        <v>64</v>
-      </c>
-      <c r="F3">
-        <v>0.1</v>
-      </c>
-      <c r="G3" t="str">
-        <f>PROPER(FALSE)</f>
-        <v>False</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="16.5">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4">
-        <v>64</v>
-      </c>
-      <c r="E4">
-        <v>64</v>
-      </c>
-      <c r="F4">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="G4" t="str">
         <f>PROPER(TRUE)</f>

</xml_diff>